<commit_message>
Started with Export feature
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -14,9 +14,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Hello world</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="23">
+  <si>
+    <t>ROOT</t>
+  </si>
+  <si>
+    <t>*150*01#</t>
+  </si>
+  <si>
+    <t>*888*01#</t>
+  </si>
+  <si>
+    <t>Send Money</t>
+  </si>
+  <si>
+    <t>Airtime &amp; Packages</t>
+  </si>
+  <si>
+    <t>Cash-Out</t>
+  </si>
+  <si>
+    <t>Pay Bills</t>
+  </si>
+  <si>
+    <t>Pay Merchant</t>
+  </si>
+  <si>
+    <t>Self Care (Account &amp; Balance)</t>
+  </si>
+  <si>
+    <t>Financial Services</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>To Mobile Number</t>
+  </si>
+  <si>
+    <t>To Contact</t>
+  </si>
+  <si>
+    <t>To Other Networks</t>
+  </si>
+  <si>
+    <t>To Other Countries</t>
+  </si>
+  <si>
+    <t>Send Money as Voucher</t>
+  </si>
+  <si>
+    <t>Receiver Number</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>PIN</t>
+  </si>
+  <si>
+    <t>USSD Flash</t>
+  </si>
+  <si>
+    <t>SMS Text</t>
+  </si>
+  <si>
+    <t>Buy Airtime</t>
+  </si>
+  <si>
+    <t>Enter Phone Number</t>
   </si>
 </sst>
 </file>
@@ -348,15 +414,628 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:H150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7">
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7">
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7">
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7">
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7">
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7">
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7">
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7">
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7">
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7">
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8">
+      <c r="G33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8">
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+      <c r="H35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8">
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8">
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8">
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8">
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8">
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8">
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8">
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8">
+      <c r="C45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8">
+      <c r="C46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8">
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8">
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="C51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3">
+      <c r="C54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="C55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="C56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3">
+      <c r="B60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3">
+      <c r="B61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3">
+      <c r="B63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3">
+      <c r="B64" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2">
+      <c r="B93" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2">
+      <c r="B95" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2">
+      <c r="B96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2">
+      <c r="B105" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2">
+      <c r="B106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2">
+      <c r="B108" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2">
+      <c r="B110" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2">
+      <c r="B111" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2">
+      <c r="B114" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2">
+      <c r="B115" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2">
+      <c r="B116" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2">
+      <c r="B117" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2">
+      <c r="B118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2">
+      <c r="B119" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2">
+      <c r="B120" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2">
+      <c r="B121" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2">
+      <c r="B122" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2">
+      <c r="B125" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2">
+      <c r="B126" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2">
+      <c r="B127" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2">
+      <c r="B128" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="B129" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="B130" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="B131" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="B132" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="B133" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="B140" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="B141" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="B142" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="C144" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3">
+      <c r="C145" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3">
+      <c r="B148" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3">
+      <c r="B149" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3">
+      <c r="B150" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New line formating, started drag-drop
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="English" sheetId="1" r:id="rId1"/>
     <sheet name="Swahili" sheetId="2" r:id="rId2"/>
+    <sheet name="Test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="34">
   <si>
     <t>ROOT</t>
   </si>
@@ -114,13 +115,17 @@
   </si>
   <si>
     <t>8. Language</t>
+  </si>
+  <si>
+    <t>CompanyName:ABC 
+ Country:India</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,8 +149,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,8 +171,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD7E4BC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -182,20 +201,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1870,4 +1903,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B4:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="4" spans="2:6">
+      <c r="B4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B4:F6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added ordering via click & refactor UIX
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -76,8 +76,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">2. Cash-Out
-3. Airtime &amp; Packages
+      <t xml:space="preserve">2. Airtime &amp; Packages
+3. Cash-Out
 4. Pay Bills
 5. Pay Merchant
 6. Self Care (Account &amp; Balance)
@@ -300,18 +300,18 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-2. Cash-Out
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">3. Airtime &amp; Packages
+2. Airtime &amp; Packages
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">3. Cash-Out
 4. Pay Bills
 5. Pay Merchant
 6. Self Care (Account &amp; Balance)
@@ -324,19 +324,19 @@
     <r>
       <t>TigoPesa
 1. Send Money
-2. Cash-Out</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3. Airtime &amp; Packages
+2. Airtime &amp; Packages</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. Cash-Out
 </t>
     </r>
     <r>
@@ -359,8 +359,8 @@
     <r>
       <t>TigoPesa
 1. Send Money
-2. Cash-Out
-3. Airtime &amp; Packages</t>
+2. Airtime &amp; Packages
+3. Cash-Out</t>
     </r>
     <r>
       <rPr>
@@ -394,8 +394,8 @@
     <r>
       <t>TigoPesa
 1. Send Money
-2. Cash-Out
-3. Airtime &amp; Packages
+2. Airtime &amp; Packages
+3. Cash-Out
 4. Pay Bills</t>
     </r>
     <r>
@@ -429,8 +429,8 @@
     <r>
       <t>TigoPesa
 1. Send Money
-2. Cash-Out
-3. Airtime &amp; Packages
+2. Airtime &amp; Packages
+3. Cash-Out
 4. Pay Bills
 5. Pay Merchant</t>
     </r>
@@ -464,8 +464,8 @@
     <r>
       <t>TigoPesa
 1. Send Money
-2. Cash-Out
-3. Airtime &amp; Packages
+2. Airtime &amp; Packages
+3. Cash-Out
 4. Pay Bills
 5. Pay Merchant
 6. Self Care (Account &amp; Balance)</t>
@@ -499,8 +499,8 @@
     <r>
       <t>TigoPesa
 1. Send Money
-2. Cash-Out
-3. Airtime &amp; Packages
+2. Airtime &amp; Packages
+3. Cash-Out
 4. Pay Bills
 5. Pay Merchant
 6. Self Care (Account &amp; Balance)
@@ -650,8 +650,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">2. Cash-Out
-3. Airtime &amp; Packages
+      <t xml:space="preserve">2. Airtime &amp; Packages
+3. Cash-Out
 4. Pay Bills
 5. Pay Merchant
 6. Self Care (Account &amp; Balance)
@@ -836,18 +836,18 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-2. Cash-Out
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">3. Airtime &amp; Packages
+2. Airtime &amp; Packages
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">3. Cash-Out
 4. Pay Bills
 5. Pay Merchant
 6. Self Care (Account &amp; Balance)
@@ -860,19 +860,19 @@
     <r>
       <t>TigoPesa
 1. Tuma Pesa
-2. Cash-Out</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3. Airtime &amp; Packages
+2. Airtime &amp; Packages</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. Cash-Out
 </t>
     </r>
     <r>
@@ -895,8 +895,8 @@
     <r>
       <t>TigoPesa
 1. Tuma Pesa
-2. Cash-Out
-3. Airtime &amp; Packages</t>
+2. Airtime &amp; Packages
+3. Cash-Out</t>
     </r>
     <r>
       <rPr>
@@ -930,8 +930,8 @@
     <r>
       <t>TigoPesa
 1. Tuma Pesa
-2. Cash-Out
-3. Airtime &amp; Packages
+2. Airtime &amp; Packages
+3. Cash-Out
 4. Pay Bills</t>
     </r>
     <r>
@@ -965,8 +965,8 @@
     <r>
       <t>TigoPesa
 1. Tuma Pesa
-2. Cash-Out
-3. Airtime &amp; Packages
+2. Airtime &amp; Packages
+3. Cash-Out
 4. Pay Bills
 5. Pay Merchant</t>
     </r>
@@ -1000,8 +1000,8 @@
     <r>
       <t>TigoPesa
 1. Tuma Pesa
-2. Cash-Out
-3. Airtime &amp; Packages
+2. Airtime &amp; Packages
+3. Cash-Out
 4. Pay Bills
 5. Pay Merchant
 6. Self Care (Account &amp; Balance)</t>
@@ -1035,8 +1035,8 @@
     <r>
       <t>TigoPesa
 1. Tuma Pesa
-2. Cash-Out
-3. Airtime &amp; Packages
+2. Airtime &amp; Packages
+3. Cash-Out
 4. Pay Bills
 5. Pay Merchant
 6. Self Care (Account &amp; Balance)

</xml_diff>